<commit_message>
1.1.0 update, added patches for 2 mods
</commit_message>
<xml_diff>
--- a/About/Rimcuisine 2 Plant distribution and stats.xlsx
+++ b/About/Rimcuisine 2 Plant distribution and stats.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\komab\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\komab\Desktop\Rimcuisine 2 Unofficial Biome Patches\About\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2761378-4946-483F-96A8-8D56791D818E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6919F4F9-53D5-4576-B399-5A00C19F3A4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3045" yWindow="600" windowWidth="15480" windowHeight="14730" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -108,9 +108,6 @@
     <t>Beetroot</t>
   </si>
   <si>
-    <t>RC2_PlantBeetroot</t>
-  </si>
-  <si>
     <t>Snap pea</t>
   </si>
   <si>
@@ -346,6 +343,9 @@
   </si>
   <si>
     <t>RC2_PlantShrooms</t>
+  </si>
+  <si>
+    <t>RC2_PlantBeet</t>
   </si>
 </sst>
 </file>
@@ -893,8 +893,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:U26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G12" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -955,34 +955,34 @@
         <v>26</v>
       </c>
       <c r="L1" s="13" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M1" s="13" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="N1" s="13" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="O1" s="13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="P1" s="13" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="Q1" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="R1" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="R1" s="13" t="s">
-        <v>41</v>
-      </c>
       <c r="S1" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="T1" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="T1" s="13" t="s">
-        <v>44</v>
-      </c>
       <c r="U1" s="14" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:21" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1325,7 +1325,7 @@
         <v>19</v>
       </c>
       <c r="G8" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H8" s="8" t="s">
         <v>21</v>
@@ -1337,37 +1337,37 @@
         <v>25</v>
       </c>
       <c r="K8" s="8" t="s">
-        <v>27</v>
+        <v>106</v>
       </c>
       <c r="L8" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="M8" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="N8" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="O8" s="8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="P8" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q8" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="Q8" s="8" t="s">
-        <v>39</v>
-      </c>
       <c r="R8" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="S8" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="T8" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="T8" s="8" t="s">
+      <c r="U8" s="9" t="s">
         <v>46</v>
-      </c>
-      <c r="U8" s="9" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="9" spans="1:21" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -1376,64 +1376,64 @@
         <v>0</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E10" s="10" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F10" s="10" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G10" s="10" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H10" s="10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I10" s="10" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J10" s="10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="K10" s="10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="L10" s="10" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="M10" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="N10" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="N10" s="10" t="s">
-        <v>74</v>
-      </c>
       <c r="O10" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="P10" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="P10" s="10" t="s">
-        <v>77</v>
-      </c>
       <c r="Q10" s="10" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="R10" s="10" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="S10" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="T10" s="10" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="U10" s="11" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="11" spans="1:21" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1721,64 +1721,64 @@
         <v>7</v>
       </c>
       <c r="B17" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="C17" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="C17" s="8" t="s">
-        <v>51</v>
-      </c>
       <c r="D17" s="8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F17" s="8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G17" s="8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H17" s="8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="I17" s="8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J17" s="8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="K17" s="8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="L17" s="8" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="M17" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="N17" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="N17" s="8" t="s">
-        <v>72</v>
-      </c>
       <c r="O17" s="8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="P17" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="Q17" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="Q17" s="8" t="s">
-        <v>79</v>
-      </c>
       <c r="R17" s="8" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="S17" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="T17" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="U17" s="9" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="18" spans="1:21" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -1787,31 +1787,31 @@
         <v>0</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H19" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="I19" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="I19" s="3" t="s">
-        <v>103</v>
-      </c>
       <c r="J19" s="4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="20" spans="1:21" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1967,31 +1967,31 @@
         <v>7</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C26" s="8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D26" s="8" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E26" s="8" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F26" s="8" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G26" s="8" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H26" s="8" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="I26" s="8" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="J26" s="9" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
   </sheetData>

</xml_diff>